<commit_message>
Elimna EC anteriores y se agregan nuevos, se modifica base de datos
</commit_message>
<xml_diff>
--- a/Data/EC/CC-45485852.xlsx
+++ b/Data/EC/CC-45485852.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\NIYARAKY\MACROS AJUSTADAS\2- MACRO COMFENALCO CARTAGENA ACTUALIZACION\Estados De Cuenta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C533F3B-8045-4B18-8C85-E43FFEF892A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE7C1FC2-5515-42D6-B1A9-6B62D65B2308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{42D49F0F-9112-4411-BB31-C14C9B7571C0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E177063B-BC14-4610-8FE0-4CF9D89B8B84}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -68,22 +68,22 @@
     <t>LEDYS DEL CARMEN RODELO VARELA</t>
   </si>
   <si>
+    <t>2505</t>
+  </si>
+  <si>
+    <t>2504</t>
+  </si>
+  <si>
+    <t>2503</t>
+  </si>
+  <si>
+    <t>2502</t>
+  </si>
+  <si>
+    <t>2501</t>
+  </si>
+  <si>
     <t>2412</t>
-  </si>
-  <si>
-    <t>2501</t>
-  </si>
-  <si>
-    <t>2502</t>
-  </si>
-  <si>
-    <t>2503</t>
-  </si>
-  <si>
-    <t>2504</t>
-  </si>
-  <si>
-    <t>2505</t>
   </si>
   <si>
     <t>2506</t>
@@ -500,7 +500,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43447FD7-909E-2BAA-6311-CFCFE96B687E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{668F4C3C-8667-4659-3C10-AB029CBC38B5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -851,7 +851,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6774CF3-82FC-4D28-899A-C1B5BDE16FAE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98B9B5D2-2944-4158-9EAF-246390E96D8B}">
   <dimension ref="B2:J28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">

</xml_diff>